<commit_message>
Info sheet should have a version for the pilot.
</commit_message>
<xml_diff>
--- a/Cost_and_Time.xlsx
+++ b/Cost_and_Time.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossspoon/PycharmProjects/short-squeeze/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65E7510F-4E10-3D4B-8E01-4CBC2F6F2821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6E6463-FF40-F845-9609-B757F9385CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{F40A4D86-4A22-6347-97F2-F0744FA3A8D1}"/>
+    <workbookView xWindow="2760" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{F40A4D86-4A22-6347-97F2-F0744FA3A8D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Max Time" sheetId="1" r:id="rId1"/>
     <sheet name="cost" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -172,7 +172,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -215,7 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6970BFE-E118-874C-9BB2-FB09FC6A8872}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,6 +705,10 @@
       <c r="B22">
         <v>120</v>
       </c>
+      <c r="C22">
+        <f>SUM(B4:B22)</f>
+        <v>3780</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -858,7 +862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838E36B1-3C42-914F-858C-317B64A2ADC0}">
   <dimension ref="A2:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>